<commit_message>
Added a few properties to excel template
</commit_message>
<xml_diff>
--- a/Documentation/user import template.xlsx
+++ b/Documentation/user import template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pixel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pixel\source\repos\MESD-Learning-Management-System\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDBE11A-9109-45DC-A263-7D47207A057C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423E8B69-7516-46D8-B1C8-906EB6EC9AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>username</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Password2023*(DON’T_CHANGE)</t>
+  </si>
+  <si>
+    <t>profile_field_nin</t>
+  </si>
+  <si>
+    <t>profile_field_phonenumber</t>
+  </si>
+  <si>
+    <t>184118929(Omang/Passport)</t>
   </si>
 </sst>
 </file>
@@ -999,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,15 +1025,17 @@
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
     <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="32.109375" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.21875" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1029,25 +1046,34 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1058,26 +1084,37 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>26776199358</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2">
+      <c r="I2" s="2">
         <v>29565</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
@@ -1090,19 +1127,19 @@
           <x14:formula1>
             <xm:f>Values!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E5</xm:sqref>
+          <xm:sqref>H2:H5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Values!$C$1:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I5</xm:sqref>
+          <xm:sqref>L2:L5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Values!$E$1:$E$17</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H4</xm:sqref>
+          <xm:sqref>K2:K4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>